<commit_message>
Fixed date and time issues
</commit_message>
<xml_diff>
--- a/Data/CaLSeN_2019.xlsx
+++ b/Data/CaLSeN_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Queer\RStudio\TickEcology\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B2718B-2649-4FBF-B224-53E7FAB20092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{408E94E1-EFDB-47B1-85FC-53352406A6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="4" xr2:uid="{0DD131C7-7A37-4803-93E2-29275B07E73D}"/>
   </bookViews>
@@ -866,10 +866,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss;@"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -958,7 +959,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1007,7 +1008,14 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1377,15 +1385,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3817EB55-A1AD-441F-9FCD-A179359C44A6}">
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="4" max="4" width="30.36328125" customWidth="1"/>
     <col min="6" max="6" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.1796875" style="11"/>
+    <col min="7" max="7" width="11.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.08984375" style="29" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1405,13 +1414,13 @@
       <c r="E1" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="27" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="6" t="s">
@@ -1483,10 +1492,10 @@
       <c r="F2" s="8">
         <v>43669</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="28">
         <v>0.46875</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="28">
         <v>0.60416666666666663</v>
       </c>
       <c r="I2" s="6">
@@ -1559,10 +1568,10 @@
       <c r="F3" s="8">
         <v>43670</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="28">
         <v>0.57638888888888895</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="28">
         <v>0.63888888888888895</v>
       </c>
       <c r="I3" s="6">
@@ -1635,10 +1644,10 @@
       <c r="F4" s="8">
         <v>43675</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="28">
         <v>0.41666666666666669</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="28">
         <v>0.5625</v>
       </c>
       <c r="I4" s="6">
@@ -1711,10 +1720,10 @@
       <c r="F5" s="8">
         <v>43669</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="28">
         <v>0.14583333333333334</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="28">
         <v>0.75</v>
       </c>
       <c r="I5" s="6">
@@ -1787,10 +1796,10 @@
       <c r="F6" s="8">
         <v>43677</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="28">
         <v>0.40625</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="28">
         <v>0.51388888888888895</v>
       </c>
       <c r="I6" s="6">
@@ -1863,10 +1872,10 @@
       <c r="F7" s="8">
         <v>43675</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="28">
         <v>0.58333333333333337</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="28">
         <v>0.72916666666666663</v>
       </c>
       <c r="I7" s="6">
@@ -1939,10 +1948,10 @@
       <c r="F8" s="8">
         <v>43670</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="28">
         <v>0.4375</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="28">
         <v>0.5</v>
       </c>
       <c r="I8" s="6">
@@ -2015,10 +2024,10 @@
       <c r="F9" s="8">
         <v>43677</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="28">
         <v>0.58333333333333337</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="28">
         <v>0.72222222222222221</v>
       </c>
       <c r="I9" s="6">
@@ -2091,10 +2100,10 @@
       <c r="F10" s="8">
         <v>43679</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="28">
         <v>0.59027777777777779</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="28">
         <v>0.70833333333333337</v>
       </c>
       <c r="I10" s="6">
@@ -2167,10 +2176,10 @@
       <c r="F11" s="8">
         <v>43669</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="28">
         <v>0.54861111111111105</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="28">
         <v>0.66666666666666663</v>
       </c>
       <c r="I11" s="6">
@@ -5190,7 +5199,7 @@
   <dimension ref="A1:P102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E106" sqref="E106"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5220,7 +5229,7 @@
       <c r="D1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="15" t="s">
         <v>158</v>
       </c>
       <c r="F1" s="18" t="s">

</xml_diff>